<commit_message>
Tela de informações completa, filtros quase completos
Tela de resultados agora está completo e foram feitos os filtros de data, falta só o de data e mm
</commit_message>
<xml_diff>
--- a/dados/dados.xlsx
+++ b/dados/dados.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mucio\Desktop\prog\Python\MannKendall\comTela\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mucio\Desktop\prog\_GitHub\Calculadora_tendencia_de_chuva\dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D03854D-A85D-4B3E-85A9-1F61BA88A15D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{078B2183-1094-4743-8638-1CF075A6AF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="dados_83423_D_1950-01-01_2023-1" sheetId="1" r:id="rId1"/>
-    <sheet name="maior 50 M e AB MAX" sheetId="7" r:id="rId2"/>
-    <sheet name="MES 3 MAIOR 50" sheetId="8" r:id="rId3"/>
-    <sheet name="1991 A 2023 MIOR 50" sheetId="9" r:id="rId4"/>
-    <sheet name="1991 A 2023" sheetId="10" r:id="rId5"/>
-    <sheet name="Mês 3 1991 a 2023" sheetId="11" r:id="rId6"/>
-    <sheet name="Planilha6" sheetId="12" r:id="rId7"/>
+    <sheet name="Teste" sheetId="13" r:id="rId2"/>
+    <sheet name="maior 50 M e AB MAX" sheetId="7" r:id="rId3"/>
+    <sheet name="MES 3 MAIOR 50" sheetId="8" r:id="rId4"/>
+    <sheet name="1991 A 2023 MIOR 50" sheetId="9" r:id="rId5"/>
+    <sheet name="1991 A 2023" sheetId="10" r:id="rId6"/>
+    <sheet name="Mês 3 1991 a 2023" sheetId="11" r:id="rId7"/>
+    <sheet name="Planilha6" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="intervalo">#REF!</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>10/011963</t>
   </si>
@@ -1583,9 +1584,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1623,7 +1624,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1729,7 +1730,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1871,7 +1872,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1882,7 +1883,7 @@
   <dimension ref="A1:B22699"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18210,6 +18211,152 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AF54FBF-615E-45EA-ABE9-A1787D1478AD}">
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>39884</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>40356</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>40548</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>41198</v>
+      </c>
+      <c r="B5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>41368</v>
+      </c>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>41869</v>
+      </c>
+      <c r="B7">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42058</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42552</v>
+      </c>
+      <c r="B9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>43048</v>
+      </c>
+      <c r="B10">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>43249</v>
+      </c>
+      <c r="B11">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>43723</v>
+      </c>
+      <c r="B12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>44185</v>
+      </c>
+      <c r="B13">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>44266</v>
+      </c>
+      <c r="B14">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>44719</v>
+      </c>
+      <c r="B15">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>45225</v>
+      </c>
+      <c r="B16">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEFEBAEC-F9AC-45B8-AB0B-44DC1AF41826}">
   <dimension ref="A1:E278"/>
   <sheetViews>
@@ -21057,7 +21204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCC5C60-96C5-4351-B667-CF7ECB8D535C}">
   <dimension ref="A1:B29"/>
   <sheetViews>
@@ -21313,7 +21460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{108DB0A4-174E-4E00-818B-0C892D20F97C}">
   <dimension ref="A1:B155"/>
   <sheetViews>
@@ -22577,7 +22724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58034726-C438-434A-BCCD-25224509318C}">
   <dimension ref="A1:B1676"/>
   <sheetViews>
@@ -36087,7 +36234,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31C9CD2-EDA0-48B4-984E-8D21683A5902}">
   <dimension ref="A1:B253"/>
   <sheetViews>
@@ -38628,7 +38775,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9913E153-7B86-43C3-91D6-E3B8E7537910}">
   <dimension ref="A1:B41"/>
   <sheetViews>
@@ -38984,12 +39131,11 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="c595b797-c883-4f42-a291-4fb33123434f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39214,11 +39360,12 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="c595b797-c883-4f42-a291-4fb33123434f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -39230,9 +39377,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF294831-E68F-4A48-8C99-D4F45E9ECAE2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{646CCC46-E1FB-4E8B-8E2E-81E410C796B7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="c595b797-c883-4f42-a291-4fb33123434f"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="4b0cdf64-be27-4828-b667-e291c2101107"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -39257,18 +39413,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{646CCC46-E1FB-4E8B-8E2E-81E410C796B7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF294831-E68F-4A48-8C99-D4F45E9ECAE2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="c595b797-c883-4f42-a291-4fb33123434f"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="4b0cdf64-be27-4828-b667-e291c2101107"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>